<commit_message>
Add GlobeSurfaceTileProvider, start implementing Camera
</commit_message>
<xml_diff>
--- a/CesiumKitStatus.xlsx
+++ b/CesiumKitStatus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="29620" yWindow="2300" windowWidth="37020" windowHeight="22540" tabRatio="500"/>
+    <workbookView xWindow="6040" yWindow="400" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1106,235 +1106,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="20">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FF3366FF"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FF9C0006"/>
-        </left>
-        <right style="thin">
-          <color rgb="FF9C0006"/>
-        </right>
-        <top style="thin">
-          <color rgb="FF9C0006"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF9C0006"/>
-        </bottom>
-      </border>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1721,8 +1493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A194" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B202" sqref="B202"/>
+    <sheetView tabSelected="1" topLeftCell="A311" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B324" sqref="B324"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4472,7 +4244,7 @@
         <v>334</v>
       </c>
       <c r="B255" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C255" t="s">
         <v>190</v>
@@ -4516,7 +4288,7 @@
         <v>252</v>
       </c>
       <c r="B259" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C259" t="s">
         <v>190</v>
@@ -4527,7 +4299,7 @@
         <v>253</v>
       </c>
       <c r="B260" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C260" t="s">
         <v>190</v>
@@ -4560,7 +4332,7 @@
         <v>256</v>
       </c>
       <c r="B263" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C263" t="s">
         <v>190</v>
@@ -4945,7 +4717,7 @@
         <v>336</v>
       </c>
       <c r="B298" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C298" t="s">
         <v>190</v>
@@ -4978,7 +4750,7 @@
         <v>339</v>
       </c>
       <c r="B301" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C301" t="s">
         <v>190</v>
@@ -5327,16 +5099,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D16:D18 B1:C1048576">
-    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="Complete">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Complete">
       <formula>NOT(ISERROR(SEARCH("Complete",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="Partial">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Partial">
       <formula>NOT(ISERROR(SEARCH("Partial",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="Not started">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Not started">
       <formula>NOT(ISERROR(SEARCH("Not started",B1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="Not porting">
+    <cfRule type="containsText" dxfId="0" priority="4" operator="containsText" text="Not porting">
       <formula>NOT(ISERROR(SEARCH("Not porting",B1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More renderer loop progress, Fixes for Xcode 6.1 Beta, unify frustum code
</commit_message>
<xml_diff>
--- a/CesiumKitStatus.xlsx
+++ b/CesiumKitStatus.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3580" yWindow="360" windowWidth="26340" windowHeight="18600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="981" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="342">
   <si>
     <t>Cesium Port Status</t>
   </si>
@@ -979,9 +979,6 @@
   </si>
   <si>
     <t>Depends on Matrix3</t>
-  </si>
-  <si>
-    <t>Interface only</t>
   </si>
   <si>
     <t>NSCopying</t>
@@ -1493,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A288" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B308" sqref="B308"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1514,10 +1511,10 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>327</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>328</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>2</v>
@@ -1638,7 +1635,7 @@
         <v>190</v>
       </c>
       <c r="D16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1652,7 +1649,7 @@
         <v>190</v>
       </c>
       <c r="D17" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1666,7 +1663,7 @@
         <v>190</v>
       </c>
       <c r="D18" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2048,7 +2045,7 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C53" t="s">
         <v>190</v>
@@ -2351,7 +2348,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="81" spans="1:4">
+    <row r="81" spans="1:3">
       <c r="A81" s="2" t="s">
         <v>78</v>
       </c>
@@ -2362,7 +2359,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="82" spans="1:4">
+    <row r="82" spans="1:3">
       <c r="A82" s="2" t="s">
         <v>79</v>
       </c>
@@ -2373,7 +2370,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="83" spans="1:4">
+    <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
         <v>80</v>
       </c>
@@ -2384,7 +2381,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="84" spans="1:4">
+    <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
         <v>81</v>
       </c>
@@ -2395,7 +2392,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="85" spans="1:4">
+    <row r="85" spans="1:3">
       <c r="A85" s="2" t="s">
         <v>82</v>
       </c>
@@ -2406,7 +2403,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="86" spans="1:4">
+    <row r="86" spans="1:3">
       <c r="A86" s="2" t="s">
         <v>83</v>
       </c>
@@ -2417,7 +2414,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="87" spans="1:4">
+    <row r="87" spans="1:3">
       <c r="A87" s="2" t="s">
         <v>84</v>
       </c>
@@ -2428,7 +2425,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="88" spans="1:4">
+    <row r="88" spans="1:3">
       <c r="A88" s="2" t="s">
         <v>85</v>
       </c>
@@ -2439,7 +2436,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="89" spans="1:4">
+    <row r="89" spans="1:3">
       <c r="A89" s="2" t="s">
         <v>86</v>
       </c>
@@ -2450,7 +2447,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="90" spans="1:4">
+    <row r="90" spans="1:3">
       <c r="A90" s="2" t="s">
         <v>87</v>
       </c>
@@ -2461,32 +2458,29 @@
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:4">
+    <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
         <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C91" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:4">
+    <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
         <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>318</v>
+        <v>191</v>
       </c>
       <c r="C92" t="s">
         <v>190</v>
       </c>
-      <c r="D92" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
+    </row>
+    <row r="93" spans="1:3">
       <c r="A93" s="2" t="s">
         <v>90</v>
       </c>
@@ -2497,7 +2491,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="94" spans="1:4">
+    <row r="94" spans="1:3">
       <c r="A94" s="2" t="s">
         <v>91</v>
       </c>
@@ -2508,7 +2502,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="95" spans="1:4">
+    <row r="95" spans="1:3">
       <c r="A95" s="2" t="s">
         <v>92</v>
       </c>
@@ -2519,7 +2513,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="96" spans="1:4">
+    <row r="96" spans="1:3">
       <c r="A96" s="2" t="s">
         <v>93</v>
       </c>
@@ -3215,7 +3209,7 @@
         <v>190</v>
       </c>
       <c r="D158" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -3229,7 +3223,7 @@
         <v>190</v>
       </c>
       <c r="D159" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -3243,7 +3237,7 @@
         <v>190</v>
       </c>
       <c r="D160" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -3323,7 +3317,7 @@
         <v>190</v>
       </c>
       <c r="D167" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -3683,7 +3677,7 @@
         <v>190</v>
       </c>
       <c r="D202" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="203" spans="1:4">
@@ -3719,7 +3713,7 @@
         <v>190</v>
       </c>
       <c r="D205" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="206" spans="1:4">
@@ -3755,10 +3749,10 @@
         <v>190</v>
       </c>
       <c r="D208" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="209" spans="1:4">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3">
       <c r="A209" t="s">
         <v>207</v>
       </c>
@@ -3769,7 +3763,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="210" spans="1:4">
+    <row r="210" spans="1:3">
       <c r="A210" t="s">
         <v>208</v>
       </c>
@@ -3780,7 +3774,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="211" spans="1:4">
+    <row r="211" spans="1:3">
       <c r="A211" t="s">
         <v>209</v>
       </c>
@@ -3791,7 +3785,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="212" spans="1:4">
+    <row r="212" spans="1:3">
       <c r="A212" t="s">
         <v>210</v>
       </c>
@@ -3802,7 +3796,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="213" spans="1:4">
+    <row r="213" spans="1:3">
       <c r="A213" t="s">
         <v>211</v>
       </c>
@@ -3813,7 +3807,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="214" spans="1:4">
+    <row r="214" spans="1:3">
       <c r="A214" t="s">
         <v>212</v>
       </c>
@@ -3824,7 +3818,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="215" spans="1:4">
+    <row r="215" spans="1:3">
       <c r="A215" t="s">
         <v>213</v>
       </c>
@@ -3835,7 +3829,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="216" spans="1:4">
+    <row r="216" spans="1:3">
       <c r="A216" t="s">
         <v>214</v>
       </c>
@@ -3846,7 +3840,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="217" spans="1:4">
+    <row r="217" spans="1:3">
       <c r="A217" t="s">
         <v>215</v>
       </c>
@@ -3857,7 +3851,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="218" spans="1:4">
+    <row r="218" spans="1:3">
       <c r="A218" t="s">
         <v>216</v>
       </c>
@@ -3867,11 +3861,8 @@
       <c r="C218" t="s">
         <v>190</v>
       </c>
-      <c r="D218" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="219" spans="1:4">
+    </row>
+    <row r="219" spans="1:3">
       <c r="A219" t="s">
         <v>217</v>
       </c>
@@ -3882,7 +3873,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="220" spans="1:4">
+    <row r="220" spans="1:3">
       <c r="A220" t="s">
         <v>218</v>
       </c>
@@ -3893,7 +3884,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="221" spans="1:4">
+    <row r="221" spans="1:3">
       <c r="A221" t="s">
         <v>219</v>
       </c>
@@ -3904,7 +3895,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="222" spans="1:4">
+    <row r="222" spans="1:3">
       <c r="A222" t="s">
         <v>220</v>
       </c>
@@ -3915,7 +3906,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="224" spans="1:4">
+    <row r="224" spans="1:3">
       <c r="A224" s="1" t="s">
         <v>221</v>
       </c>
@@ -4175,7 +4166,7 @@
     </row>
     <row r="249" spans="1:3">
       <c r="A249" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B249" t="s">
         <v>190</v>
@@ -4230,7 +4221,7 @@
     </row>
     <row r="254" spans="1:3">
       <c r="A254" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B254" t="s">
         <v>318</v>
@@ -4241,7 +4232,7 @@
     </row>
     <row r="255" spans="1:3">
       <c r="A255" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B255" t="s">
         <v>318</v>
@@ -4703,7 +4694,7 @@
     </row>
     <row r="297" spans="1:3">
       <c r="A297" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B297" t="s">
         <v>190</v>
@@ -4714,7 +4705,7 @@
     </row>
     <row r="298" spans="1:3">
       <c r="A298" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B298" t="s">
         <v>318</v>
@@ -4725,7 +4716,7 @@
     </row>
     <row r="299" spans="1:3">
       <c r="A299" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B299" t="s">
         <v>318</v>
@@ -4736,7 +4727,7 @@
     </row>
     <row r="300" spans="1:3">
       <c r="A300" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B300" t="s">
         <v>191</v>
@@ -4747,7 +4738,7 @@
     </row>
     <row r="301" spans="1:3">
       <c r="A301" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B301" t="s">
         <v>318</v>
@@ -4826,9 +4817,6 @@
       <c r="A308" t="s">
         <v>296</v>
       </c>
-      <c r="B308" t="s">
-        <v>318</v>
-      </c>
       <c r="C308" t="s">
         <v>190</v>
       </c>
@@ -5011,7 +4999,7 @@
     </row>
     <row r="325" spans="1:3">
       <c r="A325" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B325" t="s">
         <v>190</v>
@@ -5055,7 +5043,7 @@
     </row>
     <row r="329" spans="1:3">
       <c r="A329" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B329" t="s">
         <v>190</v>
@@ -5077,7 +5065,7 @@
     </row>
     <row r="331" spans="1:3">
       <c r="A331" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B331" t="s">
         <v>190</v>

</xml_diff>

<commit_message>
Build out camera support and add more tests
</commit_message>
<xml_diff>
--- a/CesiumKitStatus.xlsx
+++ b/CesiumKitStatus.xlsx
@@ -1490,8 +1490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A312" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B333" sqref="B333"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2037,7 +2037,7 @@
         <v>191</v>
       </c>
       <c r="C52" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2199,7 +2199,7 @@
         <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C67" t="s">
         <v>190</v>
@@ -2210,7 +2210,7 @@
         <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C68" t="s">
         <v>190</v>
@@ -2375,7 +2375,7 @@
         <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>190</v>
+        <v>318</v>
       </c>
       <c r="C83" t="s">
         <v>190</v>
@@ -2507,7 +2507,7 @@
         <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C95" t="s">
         <v>190</v>
@@ -2518,7 +2518,7 @@
         <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C96" t="s">
         <v>190</v>
@@ -2917,7 +2917,7 @@
         <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C132" t="s">
         <v>190</v>
@@ -3605,7 +3605,7 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C196" t="s">
         <v>190</v>
@@ -3616,7 +3616,7 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C197" t="s">
         <v>190</v>
@@ -5079,7 +5079,7 @@
         <v>317</v>
       </c>
       <c r="B332" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C332" t="s">
         <v>190</v>

</xml_diff>